<commit_message>
Finalização das suites 'Produtos' e 'Fornecedores'. Criada suite 'Vendas'
</commit_message>
<xml_diff>
--- a/Base2-SoapUi/DataSources/Produtos_DataSource.xlsx
+++ b/Base2-SoapUi/DataSources/Produtos_DataSource.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VictorPC\DevWorkspace\Base2-SoapUi\DataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="705" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="705" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="6" r:id="rId1"/>
     <sheet name="Produtos startAt endAt" sheetId="2" r:id="rId2"/>
-    <sheet name="Clientes equalTo" sheetId="3" r:id="rId3"/>
-    <sheet name="Clientes Validação de Leitura" sheetId="4" r:id="rId4"/>
-    <sheet name="Clientes Validação de Gravação" sheetId="5" r:id="rId5"/>
+    <sheet name="Produtos equalTo" sheetId="3" r:id="rId3"/>
+    <sheet name="Produtos Validação de Leitura" sheetId="4" r:id="rId4"/>
+    <sheet name="Produtos Validação de Gravação" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,67 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "sexo":"M"
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "nome": "Maria Clara Lopes" 
-}</t>
-  </si>
-  <si>
-    <t>{   
-"nome": "Maria Clara Lopes",   
- "sexo":"M" 
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "nome": "AB34567890AB34567890AB34567890AB34567890AB34567890AB34567890AB34567890AB34567890AB34567890AB345678901",
-   "sexo": "F"
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "nome": 100,
-   "sexo": "F"
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "21/10/1998",
-   "nome": "Maria Lopes",
-   "sexo": "F"
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998/10/21",
-   "nome": "Maria Lopes",
-   "sexo": "F"
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "nome": "Maria Lopes",
-   "sexo": 0
-}</t>
-  </si>
-  <si>
-    <t>{
-   "nascimento": "1998-10-21",
-   "nome": "Maria Lopes",
-   "sexo": "G"
-}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>"$key"</t>
   </si>
@@ -96,24 +36,6 @@
     <t>"nome"</t>
   </si>
   <si>
-    <t>"nascimento"</t>
-  </si>
-  <si>
-    <t>"sexo"</t>
-  </si>
-  <si>
-    <t>"1998-09-06"</t>
-  </si>
-  <si>
-    <t>"Serafina Josefa"</t>
-  </si>
-  <si>
-    <t>"F"</t>
-  </si>
-  <si>
-    <t>{"cliente10":{"nascimento":"1997-11-11","nome":"Serafina Josefa","sexo":"F"}}</t>
-  </si>
-  <si>
     <t>estoquista@teste.com</t>
   </si>
   <si>
@@ -138,22 +60,166 @@
     <t>financeiro123</t>
   </si>
   <si>
-    <t>"cliente03"</t>
-  </si>
-  <si>
-    <t>{"cliente03":{"nascimento":"1980-05-25","nome":"Jose Aparecido","sexo":"M"}}</t>
-  </si>
-  <si>
-    <t>{"cliente06":{"nascimento":"1998-09-06","nome":"Januaria Teixeira","sexo":"F"}}</t>
-  </si>
-  <si>
-    <t>{"cliente06":{"nascimento":"1998-09-06","nome":"Januaria Teixeira","sexo":"F"},"cliente10":{"nascimento":"1997-11-11","nome":"Serafina Josefa","sexo":"F"},"cliente02":{"nascimento":"1981-03-17","nome":"Joana Almeida","sexo":"F"},"cliente07":{"nascimento":"1989-09-05","nome":"Eliane Silva","sexo":"F"},"cliente08":{"nascimento":"1985-06-15","nome":"Solange Soares","sexo":"F"},"cliente05":{"nascimento":"1993-10-23","nome":"Julia de Fatima","sexo":"F"}}</t>
-  </si>
-  <si>
     <t>"produto03"</t>
   </si>
   <si>
     <t>"produto07"</t>
+  </si>
+  <si>
+    <t>{"produto06":{"descricao":"Cadeira dobravel em aço inox","marca":"Inox Movéis","nome":"Cadeira","valor":79.49},"produto05":{"descricao":"Escova de dentes grande macia","marca":"Oral-E","nome":"Escova de Dentes","valor":10.59},"produto04":{"descricao":"Camisa polo lisa ou estampada","marca":"Polo","nome":"Camisa","valor":53.99},"produto07":{"descricao":"Mesa de vidro seis lugares, luxo!","marca":"Movéis V","nome":"Mesa Seis Lugares","valor":999.9},"produto03":{"descricao":"Perfume de excelente odor","marca":"PerfEx","nome":"Perfume","valor":115.99}}</t>
+  </si>
+  <si>
+    <t>"descricao"</t>
+  </si>
+  <si>
+    <t>"Desinfetante para limpeza perfumada."</t>
+  </si>
+  <si>
+    <t>{"produto02":{"descricao":"Desinfetante para limpeza perfumada.","marca":"Desinfex","nome":"Desinfetante","valor":5.99}}</t>
+  </si>
+  <si>
+    <t>"Radio a Pilha"</t>
+  </si>
+  <si>
+    <t>{"produto01":{"descricao":"Radio a pilha para ouvir sua radio favorita em qualquer lugar.","marca":"RadioPort","nome":"Radio a Pilha","valor":50.9}}</t>
+  </si>
+  <si>
+    <t>"marca"</t>
+  </si>
+  <si>
+    <t>"Estofados Excelcior"</t>
+  </si>
+  <si>
+    <t>{"produto10":{"descricao":"Almofada de espuma grande, xadrez","marca":"Estofados Excelcior","nome":"Almofada","valor":15.99}}</t>
+  </si>
+  <si>
+    <t>"valor"</t>
+  </si>
+  <si>
+    <t>999.9</t>
+  </si>
+  <si>
+    <t>{"produto07":{"descricao":"Mesa de vidro seis lugares, luxo!","marca":"Movéis V","nome":"Mesa Seis Lugares","valor":999.9}}</t>
+  </si>
+  <si>
+    <t>"produto05"</t>
+  </si>
+  <si>
+    <t>{"produto05":{"descricao":"Escova de dentes grande macia","marca":"Oral-E","nome":"Escova de Dentes","valor":10.59}}</t>
+  </si>
+  <si>
+    <t>{
+ "nome": "Produto 11",
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "Produto 11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "Produto 11",
+ "marca": "Prod11"
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "12345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901",
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": 11,
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "12345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901",
+ "nome": "Produto 11",
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": 11,
+ "nome": "Produto 11",
+ "marca": "Prod11",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "Produto 11",
+ "marca": "12345678901234567890123456789012345678901234567890123456789012345678901234567890123456789012345678901",
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "Produto 11",
+ "marca": 11,
+ "valor": 11
+}</t>
+  </si>
+  <si>
+    <t>{
+ "descricao": "Teste do produto 11",
+ "nome": "Produto 11",
+ "marca": "Prod11",
+ "valor": "11"
+}</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t>"J"</t>
+  </si>
+  <si>
+    <t>"I"</t>
+  </si>
+  <si>
+    <t>"Z"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>"V"</t>
+  </si>
+  <si>
+    <t>{"produto06":{"descricao":"Cadeira dobravel em aço inox","marca":"Inox Movéis","nome":"Cadeira","valor":79.49},"produto04":{"descricao":"Camisa polo lisa ou estampada","marca":"Polo","nome":"Camisa","valor":53.99},"produto02":{"descricao":"Desinfetante para limpeza perfumada.","marca":"Desinfex","nome":"Desinfetante","valor":5.99},"produto05":{"descricao":"Escova de dentes grande macia","marca":"Oral-E","nome":"Escova de Dentes","valor":10.59}}</t>
+  </si>
+  <si>
+    <t>{"produto07":{"descricao":"Mesa de vidro seis lugares, luxo!","marca":"Movéis V","nome":"Mesa Seis Lugares","valor":999.9},"produto03":{"descricao":"Perfume de excelente odor","marca":"PerfEx","nome":"Perfume","valor":115.99},"produto01":{"descricao":"Radio a pilha para ouvir sua radio favorita em qualquer lugar.","marca":"RadioPort","nome":"Radio a Pilha","valor":50.9},"produto09":{"descricao":"Rodo médio para limpeza","marca":"Rodim Materias de Limpeza","nome":"Rodo","valor":23.95}}</t>
+  </si>
+  <si>
+    <t>{"produto01":{"descricao":"Radio a pilha para ouvir sua radio favorita em qualquer lugar.","marca":"RadioPort","nome":"Radio a Pilha","valor":50.9},"produto05":{"descricao":"Escova de dentes grande macia","marca":"Oral-E","nome":"Escova de Dentes","valor":10.59},"produto08":{"descricao":"Balde de plático para limpeza","marca":"Plasutilidades","nome":"Balde","valor":7.99},"produto04":{"descricao":"Camisa polo lisa ou estampada","marca":"Polo","nome":"Camisa","valor":53.99},"produto09":{"descricao":"Rodo médio para limpeza","marca":"Rodim Materias de Limpeza","nome":"Rodo","valor":23.95},"produto07":{"descricao":"Mesa de vidro seis lugares, luxo!","marca":"Movéis V","nome":"Mesa Seis Lugares","valor":999.9},"produto03":{"descricao":"Perfume de excelente odor","marca":"PerfEx","nome":"Perfume","valor":115.99}}</t>
+  </si>
+  <si>
+    <t>{"produto02":{"descricao":"Desinfetante para limpeza perfumada.","marca":"Desinfex","nome":"Desinfetante","valor":5.99},"produto01":{"descricao":"Radio a pilha para ouvir sua radio favorita em qualquer lugar.","marca":"RadioPort","nome":"Radio a Pilha","valor":50.9},"produto05":{"descricao":"Escova de dentes grande macia","marca":"Oral-E","nome":"Escova de Dentes","valor":10.59},"produto08":{"descricao":"Balde de plático para limpeza","marca":"Plasutilidades","nome":"Balde","valor":7.99},"produto10":{"descricao":"Almofada de espuma grande, xadrez","marca":"Estofados Excelcior","nome":"Almofada","valor":15.99},"produto04":{"descricao":"Camisa polo lisa ou estampada","marca":"Polo","nome":"Camisa","valor":53.99},"produto09":{"descricao":"Rodo médio para limpeza","marca":"Rodim Materias de Limpeza","nome":"Rodo","valor":23.95}}</t>
   </si>
 </sst>
 </file>
@@ -226,15 +292,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -243,10 +306,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -261,6 +320,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -543,86 +606,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,35 +696,75 @@
     <col min="4" max="4" width="73.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -669,10 +773,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,48 +786,59 @@
     <col min="3" max="3" width="70.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>27</v>
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +851,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,47 +861,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="8">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
         <v>401</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -805,7 +920,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,46 +930,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="8">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5">
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="8">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8">
-        <v>200</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
         <v>401</v>
       </c>
     </row>

</xml_diff>